<commit_message>
Reporte totales dispersion, depositos bancarios e importes totales hc
</commit_message>
<xml_diff>
--- a/Payroll/Content/REPORTES/NOMINA/HCalculo_E2001_A2021_NP11_TP3_A.xlsx
+++ b/Payroll/Content/REPORTES/NOMINA/HCalculo_E2001_A2021_NP11_TP3_A.xlsx
@@ -654,7 +654,7 @@
         <v>0</v>
       </c>
       <c r="BB2" s="10">
-        <v>3282.38</v>
+        <v>2207.38</v>
       </c>
     </row>
     <row r="3">
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="BB3" s="10">
-        <v>3747.5</v>
+        <v>2672.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>